<commit_message>
All the RFKON codes are removed into src file and standardized
</commit_message>
<xml_diff>
--- a/src/Codes.xlsx
+++ b/src/Codes.xlsx
@@ -165,7 +165,7 @@
     <t>MW5_GezKonPathPlanner_v1.1</t>
   </si>
   <si>
-    <t>Hesaplanan konumu uygulama içerisinde görselleştiren ve varış noktasına en kısa yolu tarif eden App</t>
+    <t>Hesaplanan konumu uygulama içerisinde görselleştiren ve varış noktasına en kısa yolu tarif eden App.</t>
   </si>
   <si>
     <t>Fatih'in geliştirdiği App ile konum hesaplama algoritmalarının entegrasyonu. Konsens üzerinden aktarılan mesajların (yönlendirme, uyarı, reklam, vb.) app'da bildirim olarak görselleştirilmesi.</t>
@@ -371,11 +371,11 @@
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="0" width="3"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="50.1336032388664"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="32.1376518218623"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="50.5587044534413"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="32.3481781376518"/>
     <col collapsed="false" hidden="false" max="4" min="4" style="0" width="11.1417004048583"/>
     <col collapsed="false" hidden="false" max="6" min="5" style="0" width="8.57085020242915"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="14.7813765182186"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="14.8906882591093"/>
     <col collapsed="false" hidden="false" max="1025" min="8" style="0" width="8.57085020242915"/>
   </cols>
   <sheetData>
@@ -679,16 +679,16 @@
   </sheetPr>
   <dimension ref="A1:G21"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C7" activeCellId="0" sqref="C7"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A7" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C19" activeCellId="0" sqref="C19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="0" width="3"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="33.9554655870445"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="36.7408906882591"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="20.6720647773279"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="34.2793522267206"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="37.0647773279352"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="20.7813765182186"/>
     <col collapsed="false" hidden="false" max="6" min="5" style="0" width="8.57085020242915"/>
     <col collapsed="false" hidden="false" max="7" min="7" style="0" width="10.7125506072875"/>
     <col collapsed="false" hidden="false" max="1025" min="8" style="0" width="8.57085020242915"/>
@@ -814,7 +814,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="7" customFormat="false" ht="165" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="7" customFormat="false" ht="135.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="n">
         <v>6</v>
       </c>
@@ -929,8 +929,8 @@
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="0" width="6"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="47.2388663967611"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="24.8502024291498"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="47.5627530364373"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="25.0647773279352"/>
     <col collapsed="false" hidden="false" max="4" min="4" style="0" width="11.6761133603239"/>
     <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="8.57085020242915"/>
   </cols>

</xml_diff>

<commit_message>
Preprocessed data ve Matlab kodlarında yapılan tüm değişiklikler eklendi.
</commit_message>
<xml_diff>
--- a/src/Codes.xlsx
+++ b/src/Codes.xlsx
@@ -1,18 +1,17 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="Calc"/>
-  <workbookPr backupFile="false" showObjects="all" date1904="false"/>
-  <workbookProtection/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+  <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="993"/>
   </bookViews>
   <sheets>
-    <sheet name="Matlab" sheetId="1" state="visible" r:id="rId2"/>
-    <sheet name="Mobil Cihaz + Web Service" sheetId="2" state="visible" r:id="rId3"/>
-    <sheet name="DDS" sheetId="3" state="visible" r:id="rId4"/>
+    <sheet name="Matlab" sheetId="1" r:id="rId1"/>
+    <sheet name="Mobil Cihaz + Web Service" sheetId="2" r:id="rId2"/>
+    <sheet name="DDS" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
+  <calcPr calcId="0" iterateDelta="1E-4"/>
   <extLst>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
       <loext:extCalcPr stringRefSyntax="ExcelA1"/>
@@ -22,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="67">
   <si>
     <t>Kod Adı</t>
   </si>
@@ -211,16 +210,25 @@
   </si>
   <si>
     <t>Matlab arayüzünden gelen komut setlerini sensör düğümlerine aktarıp onlardan gelen acknowledgement mesajlarını Matlab arayüzüne döndürür.</t>
+  </si>
+  <si>
+    <t>M12_SensorNodeControlPanel_v1.0</t>
+  </si>
+  <si>
+    <t>Bu app ile Matlab sunucu ile SensDug'lerin kontrolü (bağlantı açma/kapama, reset, set refresh rate/get refresh rate, get net status, get alive status) gerçeklenmektedir. Konsens sunucu ile SensDug'lerin  haberleşme işlemi TCP/IP üzerinden sağlanmaktadır.</t>
+  </si>
+  <si>
+    <t>M13_TrainRemovedNaNColumns_v1.0</t>
+  </si>
+  <si>
+    <t>Bu app ile csv formatındaki WiFi Train datasındaki ortalaması NaN içeren columnlar silinerek csv formatında NaN olmayan orijinal WiFi datasını içeren, bu NaN columnların herbir referans noktasındaki mean'lerini içeren ve bu NaN olmayan columnların headerlarının tutulduğu olmak üzere 3 tane csv dosyası üretilmektedir.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="GENERAL"/>
-  </numFmts>
-  <fonts count="5">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -229,22 +237,7 @@
       <charset val="1"/>
     </font>
     <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="0"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="0"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="0"/>
-    </font>
-    <font>
-      <b val="true"/>
+      <b/>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
@@ -252,7 +245,7 @@
       <charset val="162"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -265,9 +258,15 @@
         <bgColor rgb="FFFFFF00"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
-    <border diagonalUp="false" diagonalDown="false">
+    <border>
       <left/>
       <right/>
       <top/>
@@ -275,111 +274,368 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="20">
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+  <cellStyleXfs count="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+  </cellStyleXfs>
+  <cellXfs count="16">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="41" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-  </cellStyleXfs>
-  <cellXfs count="11">
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="14" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="6">
-    <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="false"/>
-    <cellStyle name="Comma" xfId="15" builtinId="3" customBuiltin="false"/>
-    <cellStyle name="Comma [0]" xfId="16" builtinId="6" customBuiltin="false"/>
-    <cellStyle name="Currency" xfId="17" builtinId="4" customBuiltin="false"/>
-    <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
-    <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
+  <cellStyles count="1">
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
+  <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
+<file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+  <a:themeElements>
+    <a:clrScheme name="Office">
+      <a:dk1>
+        <a:sysClr val="windowText" lastClr="000000"/>
+      </a:dk1>
+      <a:lt1>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
+      </a:lt1>
+      <a:dk2>
+        <a:srgbClr val="1F497D"/>
+      </a:dk2>
+      <a:lt2>
+        <a:srgbClr val="EEECE1"/>
+      </a:lt2>
+      <a:accent1>
+        <a:srgbClr val="4F81BD"/>
+      </a:accent1>
+      <a:accent2>
+        <a:srgbClr val="C0504D"/>
+      </a:accent2>
+      <a:accent3>
+        <a:srgbClr val="9BBB59"/>
+      </a:accent3>
+      <a:accent4>
+        <a:srgbClr val="8064A2"/>
+      </a:accent4>
+      <a:accent5>
+        <a:srgbClr val="4BACC6"/>
+      </a:accent5>
+      <a:accent6>
+        <a:srgbClr val="F79646"/>
+      </a:accent6>
+      <a:hlink>
+        <a:srgbClr val="0000FF"/>
+      </a:hlink>
+      <a:folHlink>
+        <a:srgbClr val="800080"/>
+      </a:folHlink>
+    </a:clrScheme>
+    <a:fontScheme name="Office">
+      <a:majorFont>
+        <a:latin typeface="Cambria"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Times New Roman"/>
+        <a:font script="Hebr" typeface="Times New Roman"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="MoolBoran"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Times New Roman"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+      </a:majorFont>
+      <a:minorFont>
+        <a:latin typeface="Calibri"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Arial"/>
+        <a:font script="Hebr" typeface="Arial"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="DaunPenh"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Arial"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+      </a:minorFont>
+    </a:fontScheme>
+    <a:fmtScheme name="Office">
+      <a:fillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="50000"/>
+                <a:satMod val="300000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="35000">
+              <a:schemeClr val="phClr">
+                <a:tint val="37000"/>
+                <a:satMod val="300000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:tint val="15000"/>
+                <a:satMod val="350000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="16200000" scaled="1"/>
+        </a:gradFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:shade val="51000"/>
+                <a:satMod val="130000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="80000">
+              <a:schemeClr val="phClr">
+                <a:shade val="93000"/>
+                <a:satMod val="130000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="94000"/>
+                <a:satMod val="135000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="16200000" scaled="0"/>
+        </a:gradFill>
+      </a:fillStyleLst>
+      <a:lnStyleLst>
+        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr">
+              <a:shade val="95000"/>
+              <a:satMod val="105000"/>
+            </a:schemeClr>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+        </a:ln>
+        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+        </a:ln>
+        <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+        </a:ln>
+      </a:lnStyleLst>
+      <a:effectStyleLst>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="40000" dist="20000" dir="5400000" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="38000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="35000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="35000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+          <a:scene3d>
+            <a:camera prst="orthographicFront">
+              <a:rot lat="0" lon="0" rev="0"/>
+            </a:camera>
+            <a:lightRig rig="threePt" dir="t">
+              <a:rot lat="0" lon="0" rev="1200000"/>
+            </a:lightRig>
+          </a:scene3d>
+          <a:sp3d>
+            <a:bevelT w="63500" h="25400"/>
+          </a:sp3d>
+        </a:effectStyle>
+      </a:effectStyleLst>
+      <a:bgFillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="40000"/>
+                <a:satMod val="350000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="40000">
+              <a:schemeClr val="phClr">
+                <a:tint val="45000"/>
+                <a:shade val="99000"/>
+                <a:satMod val="350000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="20000"/>
+                <a:satMod val="255000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:path path="circle">
+            <a:fillToRect l="50000" t="-80000" r="50000" b="180000"/>
+          </a:path>
+        </a:gradFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="80000"/>
+                <a:satMod val="300000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="30000"/>
+                <a:satMod val="200000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:path path="circle">
+            <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
+          </a:path>
+        </a:gradFill>
+      </a:bgFillStyleLst>
+    </a:fmtScheme>
+  </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
+</a:theme>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
-  <dimension ref="A1:H20"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:H14"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C11" activeCellId="0" sqref="C11"/>
+    <sheetView tabSelected="1" topLeftCell="A14" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B23" sqref="B23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="3"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="50.5587044534413"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="32.3481781376518"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="11.1417004048583"/>
-    <col collapsed="false" hidden="false" max="6" min="5" style="0" width="8.57085020242915"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="14.8906882591093"/>
-    <col collapsed="false" hidden="false" max="1025" min="8" style="0" width="8.57085020242915"/>
+    <col min="1" max="1" width="3"/>
+    <col min="2" max="2" width="50.5703125"/>
+    <col min="3" max="3" width="32.28515625" style="1"/>
+    <col min="4" max="4" width="11.140625"/>
+    <col min="5" max="5" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="8.5703125"/>
+    <col min="7" max="7" width="14.85546875"/>
+    <col min="8" max="1025" width="8.5703125"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B1" s="2" t="s">
         <v>0</v>
       </c>
@@ -400,8 +656,8 @@
       </c>
       <c r="H1" s="2"/>
     </row>
-    <row r="2" customFormat="false" ht="75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="4" t="n">
+    <row r="2" spans="1:8" ht="75" x14ac:dyDescent="0.25">
+      <c r="A2" s="4">
         <v>1</v>
       </c>
       <c r="B2" s="5" t="s">
@@ -421,51 +677,53 @@
         <v>10</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="n">
+    <row r="3" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+      <c r="A3" s="11">
         <v>2</v>
       </c>
-      <c r="B3" s="0" t="s">
+      <c r="B3" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="C3" s="8" t="s">
+      <c r="C3" s="14" t="s">
         <v>12</v>
       </c>
-      <c r="D3" s="9" t="s">
-        <v>8</v>
-      </c>
-      <c r="F3" s="0" t="s">
-        <v>9</v>
-      </c>
-      <c r="G3" s="0" t="s">
+      <c r="D3" s="15" t="s">
+        <v>8</v>
+      </c>
+      <c r="E3" s="11"/>
+      <c r="F3" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="G3" s="11" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="60" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="0" t="n">
+    <row r="4" spans="1:8" ht="60" x14ac:dyDescent="0.25">
+      <c r="A4" s="11">
         <v>3</v>
       </c>
-      <c r="B4" s="0" t="s">
+      <c r="B4" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="C4" s="8" t="s">
+      <c r="C4" s="14" t="s">
         <v>14</v>
       </c>
-      <c r="D4" s="9" t="s">
-        <v>8</v>
-      </c>
-      <c r="F4" s="0" t="s">
-        <v>9</v>
-      </c>
-      <c r="G4" s="0" t="s">
+      <c r="D4" s="15" t="s">
+        <v>8</v>
+      </c>
+      <c r="E4" s="11"/>
+      <c r="F4" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="G4" s="11" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="90" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="0" t="n">
+    <row r="5" spans="1:8" ht="90" x14ac:dyDescent="0.25">
+      <c r="A5">
         <v>4</v>
       </c>
-      <c r="B5" s="0" t="s">
+      <c r="B5" t="s">
         <v>15</v>
       </c>
       <c r="C5" s="8" t="s">
@@ -474,18 +732,18 @@
       <c r="D5" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="F5" s="0" t="s">
+      <c r="F5" t="s">
         <v>9</v>
       </c>
       <c r="G5" s="9" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="6" customFormat="false" ht="105" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="0" t="n">
+    <row r="6" spans="1:8" ht="105" x14ac:dyDescent="0.25">
+      <c r="A6">
         <v>5</v>
       </c>
-      <c r="B6" s="0" t="s">
+      <c r="B6" t="s">
         <v>18</v>
       </c>
       <c r="C6" s="8" t="s">
@@ -501,51 +759,53 @@
         <v>17</v>
       </c>
     </row>
-    <row r="7" customFormat="false" ht="45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="0" t="n">
+    <row r="7" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+      <c r="A7" s="11">
         <v>6</v>
       </c>
-      <c r="B7" s="0" t="s">
+      <c r="B7" s="11" t="s">
         <v>20</v>
       </c>
-      <c r="C7" s="8" t="s">
+      <c r="C7" s="14" t="s">
         <v>21</v>
       </c>
-      <c r="D7" s="9" t="s">
-        <v>8</v>
-      </c>
-      <c r="F7" s="0" t="s">
-        <v>9</v>
-      </c>
-      <c r="G7" s="9" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="8" customFormat="false" ht="60" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="0" t="n">
+      <c r="D7" s="15" t="s">
+        <v>8</v>
+      </c>
+      <c r="E7" s="11"/>
+      <c r="F7" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="G7" s="15" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" ht="60" x14ac:dyDescent="0.25">
+      <c r="A8" s="11">
         <v>7</v>
       </c>
-      <c r="B8" s="0" t="s">
+      <c r="B8" s="11" t="s">
         <v>22</v>
       </c>
-      <c r="C8" s="8" t="s">
+      <c r="C8" s="14" t="s">
         <v>23</v>
       </c>
-      <c r="D8" s="9" t="s">
-        <v>8</v>
-      </c>
-      <c r="F8" s="0" t="s">
-        <v>9</v>
-      </c>
-      <c r="G8" s="9" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="9" customFormat="false" ht="90" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="0" t="n">
-        <v>8</v>
-      </c>
-      <c r="B9" s="0" t="s">
+      <c r="D8" s="15" t="s">
+        <v>8</v>
+      </c>
+      <c r="E8" s="11"/>
+      <c r="F8" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="G8" s="15" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" ht="90" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>8</v>
+      </c>
+      <c r="B9" t="s">
         <v>24</v>
       </c>
       <c r="C9" s="8" t="s">
@@ -554,18 +814,18 @@
       <c r="D9" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="F9" s="0" t="s">
+      <c r="F9" t="s">
         <v>9</v>
       </c>
       <c r="G9" s="9" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="10" customFormat="false" ht="90" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="0" t="n">
-        <v>9</v>
-      </c>
-      <c r="B10" s="0" t="s">
+    <row r="10" spans="1:8" ht="90" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>9</v>
+      </c>
+      <c r="B10" t="s">
         <v>26</v>
       </c>
       <c r="C10" s="8" t="s">
@@ -574,38 +834,39 @@
       <c r="D10" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="F10" s="0" t="s">
+      <c r="F10" t="s">
         <v>9</v>
       </c>
       <c r="G10" s="9" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="11" customFormat="false" ht="90" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="0" t="n">
+    <row r="11" spans="1:8" ht="90" x14ac:dyDescent="0.25">
+      <c r="A11" s="11">
         <v>10</v>
       </c>
-      <c r="B11" s="0" t="s">
+      <c r="B11" s="11" t="s">
         <v>28</v>
       </c>
-      <c r="C11" s="8" t="s">
+      <c r="C11" s="14" t="s">
         <v>29</v>
       </c>
-      <c r="D11" s="9" t="s">
-        <v>8</v>
-      </c>
-      <c r="F11" s="0" t="s">
-        <v>9</v>
-      </c>
-      <c r="G11" s="9" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="12" customFormat="false" ht="45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="0" t="n">
+      <c r="D11" s="15" t="s">
+        <v>8</v>
+      </c>
+      <c r="E11" s="11"/>
+      <c r="F11" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="G11" s="15" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+      <c r="A12">
         <v>11</v>
       </c>
-      <c r="B12" s="0" t="s">
+      <c r="B12" t="s">
         <v>30</v>
       </c>
       <c r="C12" s="8" t="s">
@@ -614,87 +875,83 @@
       <c r="D12" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="F12" s="0" t="s">
+      <c r="F12" t="s">
         <v>9</v>
       </c>
       <c r="G12" s="9" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="0" t="n">
+    <row r="13" spans="1:8" ht="135" x14ac:dyDescent="0.25">
+      <c r="A13" s="11">
         <v>12</v>
       </c>
-    </row>
-    <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="0" t="n">
+      <c r="B13" s="11" t="s">
+        <v>63</v>
+      </c>
+      <c r="C13" s="12" t="s">
+        <v>64</v>
+      </c>
+      <c r="D13" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="E13" s="13">
+        <v>42415</v>
+      </c>
+      <c r="F13" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="G13" s="11" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" ht="165" x14ac:dyDescent="0.25">
+      <c r="A14" s="11">
         <v>13</v>
       </c>
-    </row>
-    <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="0" t="n">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="0" t="n">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="0" t="n">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="0" t="n">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="0" t="n">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="0" t="n">
-        <v>19</v>
+      <c r="B14" s="11" t="s">
+        <v>65</v>
+      </c>
+      <c r="C14" s="12" t="s">
+        <v>66</v>
+      </c>
+      <c r="D14" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="E14" s="11"/>
+      <c r="F14" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="G14" s="11" t="s">
+        <v>10</v>
       </c>
     </row>
   </sheetData>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
-    <oddFooter/>
-  </headerFooter>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
+  <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G21"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A7" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C19" activeCellId="0" sqref="C19"/>
+    <sheetView topLeftCell="A7" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="3"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="34.2793522267206"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="37.0647773279352"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="20.7813765182186"/>
-    <col collapsed="false" hidden="false" max="6" min="5" style="0" width="8.57085020242915"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="10.7125506072875"/>
-    <col collapsed="false" hidden="false" max="1025" min="8" style="0" width="8.57085020242915"/>
+    <col min="1" max="1" width="3"/>
+    <col min="2" max="2" width="34.28515625"/>
+    <col min="3" max="3" width="37"/>
+    <col min="4" max="4" width="20.7109375"/>
+    <col min="5" max="6" width="8.5703125"/>
+    <col min="7" max="7" width="10.7109375"/>
+    <col min="8" max="1025" width="8.5703125"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B1" s="2" t="s">
         <v>0</v>
       </c>
@@ -714,51 +971,51 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="88.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="n">
+    <row r="2" spans="1:7" ht="88.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2">
         <v>1</v>
       </c>
-      <c r="B2" s="0" t="s">
+      <c r="B2" t="s">
         <v>32</v>
       </c>
       <c r="C2" s="8" t="s">
         <v>33</v>
       </c>
-      <c r="D2" s="0" t="s">
+      <c r="D2" t="s">
         <v>34</v>
       </c>
-      <c r="F2" s="0" t="s">
+      <c r="F2" t="s">
         <v>35</v>
       </c>
       <c r="G2" s="9" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="123.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="n">
+    <row r="3" spans="1:7" ht="123.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3">
         <v>2</v>
       </c>
-      <c r="B3" s="0" t="s">
+      <c r="B3" t="s">
         <v>36</v>
       </c>
       <c r="C3" s="8" t="s">
         <v>37</v>
       </c>
-      <c r="D3" s="0" t="s">
+      <c r="D3" t="s">
         <v>34</v>
       </c>
-      <c r="F3" s="0" t="s">
+      <c r="F3" t="s">
         <v>38</v>
       </c>
       <c r="G3" s="9" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="133.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A4" s="0" t="n">
+    <row r="4" spans="1:7" ht="133.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4">
         <v>3</v>
       </c>
-      <c r="B4" s="0" t="s">
+      <c r="B4" t="s">
         <v>39</v>
       </c>
       <c r="C4" s="8" t="s">
@@ -767,58 +1024,58 @@
       <c r="D4" s="8" t="s">
         <v>41</v>
       </c>
-      <c r="F4" s="0" t="s">
+      <c r="F4" t="s">
         <v>35</v>
       </c>
       <c r="G4" s="9" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="0" t="n">
+    <row r="5" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A5">
         <v>4</v>
       </c>
-      <c r="B5" s="0" t="s">
+      <c r="B5" t="s">
         <v>42</v>
       </c>
       <c r="C5" s="8" t="s">
         <v>43</v>
       </c>
-      <c r="D5" s="0" t="s">
+      <c r="D5" t="s">
         <v>34</v>
       </c>
-      <c r="F5" s="0" t="s">
+      <c r="F5" t="s">
         <v>35</v>
       </c>
       <c r="G5" s="9" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="6" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="0" t="n">
+    <row r="6" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A6">
         <v>5</v>
       </c>
-      <c r="B6" s="0" t="s">
+      <c r="B6" t="s">
         <v>44</v>
       </c>
       <c r="C6" s="8" t="s">
         <v>45</v>
       </c>
-      <c r="D6" s="0" t="s">
+      <c r="D6" t="s">
         <v>34</v>
       </c>
-      <c r="F6" s="0" t="s">
+      <c r="F6" t="s">
         <v>35</v>
       </c>
       <c r="G6" s="9" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="7" customFormat="false" ht="135.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="0" t="n">
+    <row r="7" spans="1:7" ht="165" x14ac:dyDescent="0.25">
+      <c r="A7">
         <v>6</v>
       </c>
-      <c r="B7" s="0" t="s">
+      <c r="B7" t="s">
         <v>46</v>
       </c>
       <c r="C7" s="8" t="s">
@@ -827,115 +1084,107 @@
       <c r="D7" s="10" t="s">
         <v>48</v>
       </c>
-      <c r="F7" s="0" t="s">
+      <c r="F7" t="s">
         <v>35</v>
       </c>
       <c r="G7" s="9" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="0" t="n">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8">
         <v>7</v>
       </c>
     </row>
-    <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="0" t="n">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="0" t="n">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="0" t="n">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A11">
         <v>10</v>
       </c>
     </row>
-    <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="0" t="n">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A12">
         <v>11</v>
       </c>
     </row>
-    <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="0" t="n">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A13">
         <v>12</v>
       </c>
     </row>
-    <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="0" t="n">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A14">
         <v>13</v>
       </c>
     </row>
-    <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="0" t="n">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A15">
         <v>14</v>
       </c>
     </row>
-    <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="0" t="n">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A16">
         <v>15</v>
       </c>
     </row>
-    <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="0" t="n">
+    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A17">
         <v>16</v>
       </c>
     </row>
-    <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="0" t="n">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="0" t="n">
+    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A19">
         <v>18</v>
       </c>
     </row>
-    <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="0" t="n">
+    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A20">
         <v>19</v>
       </c>
     </row>
-    <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="0" t="n">
+    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A21">
         <v>20</v>
       </c>
     </row>
   </sheetData>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
-    <oddFooter/>
-  </headerFooter>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
+  <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G14"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A4" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H8" activeCellId="0" sqref="H8"/>
+    <sheetView topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H8" sqref="H8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="6"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="47.5627530364373"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="25.0647773279352"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="11.6761133603239"/>
-    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="8.57085020242915"/>
+    <col min="1" max="1" width="6"/>
+    <col min="2" max="2" width="47.5703125"/>
+    <col min="3" max="3" width="25"/>
+    <col min="4" max="4" width="11.7109375"/>
+    <col min="5" max="1025" width="8.5703125"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B1" s="2" t="s">
         <v>0</v>
       </c>
@@ -955,183 +1204,178 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="66" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="n">
+    <row r="2" spans="1:7" ht="66" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2">
         <v>1</v>
       </c>
-      <c r="B2" s="0" t="s">
+      <c r="B2" t="s">
         <v>49</v>
       </c>
       <c r="C2" s="8" t="s">
         <v>50</v>
       </c>
-      <c r="D2" s="0" t="s">
+      <c r="D2" t="s">
         <v>34</v>
       </c>
-      <c r="F2" s="0" t="s">
+      <c r="F2" t="s">
         <v>35</v>
       </c>
-      <c r="G2" s="0" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="3" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="n">
+      <c r="G2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A3">
         <v>2</v>
       </c>
-      <c r="B3" s="0" t="s">
+      <c r="B3" t="s">
         <v>51</v>
       </c>
       <c r="C3" s="8" t="s">
         <v>52</v>
       </c>
-      <c r="D3" s="0" t="s">
+      <c r="D3" t="s">
         <v>34</v>
       </c>
-      <c r="F3" s="0" t="s">
+      <c r="F3" t="s">
         <v>35</v>
       </c>
-      <c r="G3" s="0" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="4" customFormat="false" ht="60" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="0" t="n">
+      <c r="G3" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+      <c r="A4">
         <v>3</v>
       </c>
-      <c r="B4" s="0" t="s">
+      <c r="B4" t="s">
         <v>53</v>
       </c>
       <c r="C4" s="8" t="s">
         <v>54</v>
       </c>
-      <c r="D4" s="0" t="s">
+      <c r="D4" t="s">
         <v>34</v>
       </c>
-      <c r="F4" s="0" t="s">
+      <c r="F4" t="s">
         <v>35</v>
       </c>
-      <c r="G4" s="0" t="s">
+      <c r="G4" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="0" t="n">
+    <row r="5" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="A5">
         <v>4</v>
       </c>
-      <c r="B5" s="0" t="s">
+      <c r="B5" t="s">
         <v>55</v>
       </c>
       <c r="C5" s="8" t="s">
         <v>56</v>
       </c>
-      <c r="D5" s="0" t="s">
+      <c r="D5" t="s">
         <v>34</v>
       </c>
-      <c r="F5" s="0" t="s">
+      <c r="F5" t="s">
         <v>35</v>
       </c>
-      <c r="G5" s="0" t="s">
+      <c r="G5" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="6" customFormat="false" ht="60" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="0" t="n">
+    <row r="6" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+      <c r="A6">
         <v>5</v>
       </c>
-      <c r="B6" s="0" t="s">
+      <c r="B6" t="s">
         <v>57</v>
       </c>
       <c r="C6" s="8" t="s">
         <v>58</v>
       </c>
-      <c r="D6" s="0" t="s">
+      <c r="D6" t="s">
         <v>34</v>
       </c>
-      <c r="F6" s="0" t="s">
+      <c r="F6" t="s">
         <v>35</v>
       </c>
-      <c r="G6" s="0" t="s">
+      <c r="G6" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="7" customFormat="false" ht="45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="0" t="n">
+    <row r="7" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="A7">
         <v>6</v>
       </c>
-      <c r="B7" s="0" t="s">
+      <c r="B7" t="s">
         <v>59</v>
       </c>
       <c r="C7" s="8" t="s">
         <v>60</v>
       </c>
-      <c r="D7" s="0" t="s">
+      <c r="D7" t="s">
         <v>34</v>
       </c>
-      <c r="F7" s="0" t="s">
+      <c r="F7" t="s">
         <v>35</v>
       </c>
-      <c r="G7" s="0" t="s">
+      <c r="G7" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="8" customFormat="false" ht="105" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="0" t="n">
+    <row r="8" spans="1:7" ht="105" x14ac:dyDescent="0.25">
+      <c r="A8">
         <v>7</v>
       </c>
-      <c r="B8" s="0" t="s">
+      <c r="B8" t="s">
         <v>61</v>
       </c>
       <c r="C8" s="8" t="s">
         <v>62</v>
       </c>
-      <c r="D8" s="0" t="s">
+      <c r="D8" t="s">
         <v>34</v>
       </c>
-      <c r="F8" s="0" t="s">
+      <c r="F8" t="s">
         <v>35</v>
       </c>
-      <c r="G8" s="0" t="s">
+      <c r="G8" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="0" t="n">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="0" t="n">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="0" t="n">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A11">
         <v>10</v>
       </c>
     </row>
-    <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="0" t="n">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A12">
         <v>11</v>
       </c>
     </row>
-    <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="0" t="n">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A13">
         <v>12</v>
       </c>
     </row>
-    <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="0" t="n">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A14">
         <v>13</v>
       </c>
     </row>
   </sheetData>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
-    <oddFooter/>
-  </headerFooter>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
+  <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
 </worksheet>
 </file>
</xml_diff>